<commit_message>
Update use NPOI over EPPLUS to support old version of excel
</commit_message>
<xml_diff>
--- a/TestConsole/File/TestFile.xlsx
+++ b/TestConsole/File/TestFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rayra\source\repos\syntaxerror00100\FluentExcelValidator\TestConsole\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362FC2A1-060B-4C1A-9E41-339CE0BC7528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B136319-BA89-4C5E-B458-BDBF3979CE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="5940" windowWidth="37530" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>First Name</t>
   </si>
@@ -195,13 +195,22 @@
   </si>
   <si>
     <t>Ignored column</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>email@gmail.com</t>
+  </si>
+  <si>
+    <t>email.invalid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +230,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -239,13 +256,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -259,10 +279,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,9 +555,10 @@
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,162 +568,225 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="C22" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -714,33 +794,47 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="C24" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="C25" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="C26" t="s">
         <v>47</v>
       </c>
+      <c r="D26" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{7DA45D55-E761-426B-B239-D1AFC2F94B11}"/>
+    <hyperlink ref="D5:D22" r:id="rId2" display="email@gmail.com" xr:uid="{68DC1F4B-8E5E-4D24-AD64-F7457276ED77}"/>
+    <hyperlink ref="D24:D26" r:id="rId3" display="email@gmail.com" xr:uid="{4065E70C-1E5B-497A-A9BB-EEC88E65A7A6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>